<commit_message>
cleaning folders (putting outputs inside legacy folder)
</commit_message>
<xml_diff>
--- a/Documentation/mina-finalResults-graphs.xlsx
+++ b/Documentation/mina-finalResults-graphs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitRepos\Internship_RuG_2020\mina-completeCycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitRepos\Internship_RuG_2020\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3843A5E3-115F-4C91-AF66-B7D92029EC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7437E232-EF2F-4720-A4F8-64038BF01643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mina-finalResults-CSV" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,10 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'mina-finalResults-CSV'!$J$13:$J$293</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'mina-finalResults-CSV'!$J$2:$J$12</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'mina-finalResults-CSV'!$J$13:$J$293</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'mina-finalResults-CSV'!$J$2:$J$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3704,7 +3702,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[mina-finalResults.xlsx]Graphs and Tables!PivotTable6</c:name>
+    <c:name>[mina-finalResults-graphs.xlsx]Graphs and Tables!PivotTable6</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -7269,8 +7267,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4976877" y="12702669"/>
-              <a:ext cx="6890556" cy="3978088"/>
+              <a:off x="4971434" y="12702669"/>
+              <a:ext cx="6875588" cy="3978088"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7904,9 +7902,9 @@
     <cacheField name="Visitor" numFmtId="1">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="SumOfPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns + ABS(NumberOfRemovedPatterns )" databaseField="0"/>
-    <cacheField name="TotalPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns + ABS(NumberOfRemovedPatterns )" databaseField="0"/>
-    <cacheField name="AbsoluteRemovedPatterns" numFmtId="0" formula="ABS(NumberOfRemovedPatterns )" databaseField="0"/>
+    <cacheField name="SumOfPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
+    <cacheField name="TotalPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
+    <cacheField name="AbsoluteRemovedPatterns" numFmtId="0" formula="ABS(NumberOfRemovedPatterns)" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -16974,7 +16972,238 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="32">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
+      <items count="11">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Sum of AbsoluteRemovedPatterns" fld="31" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B92:E98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="32">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Sum of NumberOfRemovedPatterns" fld="11" baseField="0" baseItem="0"/>
+    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B71:C77" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="32">
     <pivotField showAll="0"/>
@@ -17061,8 +17290,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="B57:D66" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="32">
     <pivotField showAll="0"/>
@@ -17559,237 +17788,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="32">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
-      <items count="11">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of AbsoluteRemovedPatterns" fld="31" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B92:E98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="32">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of NumberOfRemovedPatterns" fld="11" baseField="0" baseItem="0"/>
-    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AC293" totalsRowShown="0">
   <autoFilter ref="A1:AC293" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -18138,34 +18136,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC293"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB44" sqref="AB44"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="128" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="113.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22" customWidth="1"/>
-    <col min="24" max="24" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -31293,7 +31298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes to presentation and small change to graph on xlsx
</commit_message>
<xml_diff>
--- a/Documentation/mina-finalResults-graphs.xlsx
+++ b/Documentation/mina-finalResults-graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitRepos\Internship_RuG_2020\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7437E232-EF2F-4720-A4F8-64038BF01643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3409B0-8B83-48B8-90F8-B69DE57BB396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mina-finalResults-CSV" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2359,9 +2359,6 @@
     <t>Sum of NumberOfAddedPatterns</t>
   </si>
   <si>
-    <t>Sum of NumberOfRemovedPatterns</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -2390,6 +2387,9 @@
   </si>
   <si>
     <t>Sum of AbsoluteRemovedPatterns</t>
+  </si>
+  <si>
+    <t>Sum of NumberOfRemovedPatterns(Absolute)</t>
   </si>
 </sst>
 </file>
@@ -3046,10 +3046,7 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -3100,7 +3097,10 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7414,7 +7414,7 @@
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="32">
+  <cacheFields count="33">
     <cacheField name="Project" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -7905,6 +7905,7 @@
     <cacheField name="SumOfPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
     <cacheField name="TotalPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
     <cacheField name="AbsoluteRemovedPatterns" numFmtId="0" formula="ABS(NumberOfRemovedPatterns)" databaseField="0"/>
+    <cacheField name="NumberOfRemovedPatterns(Absolute)" numFmtId="0" formula=" ABS(NumberOfRemovedPatterns )" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -16972,240 +16973,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="32">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
-      <items count="11">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of AbsoluteRemovedPatterns" fld="31" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B92:E98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="32">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of NumberOfRemovedPatterns" fld="11" baseField="0" baseItem="0"/>
-    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B71:C77" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="32">
+  <pivotFields count="33">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -17245,6 +17015,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -17290,10 +17061,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="B57:D66" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="32">
+  <pivotFields count="33">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
       <items count="293">
@@ -17728,6 +17499,7 @@
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="2"/>
@@ -17788,6 +17560,239 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="33">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
+      <items count="11">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Sum of AbsoluteRemovedPatterns" fld="31" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B92:E98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="33">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Sum of NumberOfRemovedPatterns(Absolute)" fld="32" baseField="0" baseItem="0"/>
+    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AC293" totalsRowShown="0">
   <autoFilter ref="A1:AC293" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -17804,23 +17809,23 @@
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="TimeToResolve(Days)"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NumberOfAddedPatterns"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NumberOfRemovedPatterns"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Abstract Factory" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Factory Method" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Singleton" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Adapter" dataDxfId="15"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Bridge" dataDxfId="14"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Composite" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Decorator" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Facade" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Flyweight" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Proxy" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Chain of Responsibility" dataDxfId="8"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Mediator" dataDxfId="7"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Observer" dataDxfId="6"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="State" dataDxfId="5"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Strategy" dataDxfId="4"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Template Method" dataDxfId="3"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Visitor" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Abstract Factory" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Factory Method" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Singleton" dataDxfId="14"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Adapter" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Bridge" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Composite" dataDxfId="11"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Decorator" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Facade" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Flyweight" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Proxy" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Chain of Responsibility" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Mediator" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Observer" dataDxfId="4"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="State" dataDxfId="3"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Strategy" dataDxfId="2"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Template Method" dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Visitor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17830,8 +17835,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00C4A24C-F4A7-4272-A428-C9904738F93F}" name="Table3" displayName="Table3" ref="E57:F65" totalsRowShown="0">
   <autoFilter ref="E57:F65" xr:uid="{EB3308BB-A406-42BA-A76D-F94720BFCCA3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CB378E6D-067E-4D65-BC80-38A6B0CE5641}" name="Count of CommitID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{9C45E57F-72E8-4004-9367-2BB9F710DAA0}" name="PatternChanges" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CB378E6D-067E-4D65-BC80-38A6B0CE5641}" name="Count of CommitID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{9C45E57F-72E8-4004-9367-2BB9F710DAA0}" name="PatternChanges" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18136,8 +18141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31298,16 +31303,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:S98"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -31381,7 +31387,7 @@
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C3" s="6">
         <f>SUMIF(Table1[Abstract Factory],"&gt;0")</f>
@@ -31454,7 +31460,7 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C4" s="8">
         <f>ABS(SUMIF(Table1[Abstract Factory],"&lt;0"))</f>
@@ -31527,7 +31533,7 @@
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C5" s="8" t="e">
         <f>C3/C7*100</f>
@@ -31600,7 +31606,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C6" s="8" t="e">
         <f>C4/C7*100</f>
@@ -31673,7 +31679,7 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C7" s="9">
         <f t="shared" ref="C7:S7" si="2">C3+C4</f>
@@ -31759,7 +31765,7 @@
         <v>772</v>
       </c>
       <c r="D33" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -31866,16 +31872,16 @@
         <v>770</v>
       </c>
       <c r="C57" t="s">
+        <v>778</v>
+      </c>
+      <c r="D57" t="s">
         <v>779</v>
       </c>
-      <c r="D57" t="s">
-        <v>780</v>
-      </c>
       <c r="E57" t="s">
+        <v>778</v>
+      </c>
+      <c r="F57" t="s">
         <v>779</v>
-      </c>
-      <c r="F57" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -32030,7 +32036,7 @@
         <v>770</v>
       </c>
       <c r="C71" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
@@ -32089,10 +32095,10 @@
         <v>772</v>
       </c>
       <c r="D92" t="s">
-        <v>773</v>
+        <v>783</v>
       </c>
       <c r="E92" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
@@ -32103,7 +32109,7 @@
         <v>51</v>
       </c>
       <c r="D93" s="4">
-        <v>-43</v>
+        <v>43</v>
       </c>
       <c r="E93" s="4">
         <v>94</v>
@@ -32117,7 +32123,7 @@
         <v>86</v>
       </c>
       <c r="D94" s="4">
-        <v>-96</v>
+        <v>96</v>
       </c>
       <c r="E94" s="4">
         <v>182</v>
@@ -32131,7 +32137,7 @@
         <v>157</v>
       </c>
       <c r="D95" s="4">
-        <v>-80</v>
+        <v>80</v>
       </c>
       <c r="E95" s="4">
         <v>237</v>
@@ -32145,7 +32151,7 @@
         <v>32</v>
       </c>
       <c r="D96" s="4">
-        <v>-41</v>
+        <v>41</v>
       </c>
       <c r="E96" s="4">
         <v>73</v>
@@ -32173,7 +32179,7 @@
         <v>328</v>
       </c>
       <c r="D98" s="4">
-        <v>-260</v>
+        <v>260</v>
       </c>
       <c r="E98" s="4">
         <v>588</v>

</xml_diff>

<commit_message>
added final changes to scripts (to comply with new naming), new versions of the figures in the Documentation folder and added better analysis to the excel file
</commit_message>
<xml_diff>
--- a/Documentation/mina-finalResults-graphs.xlsx
+++ b/Documentation/mina-finalResults-graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitRepos\Internship_RuG_2020\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3409B0-8B83-48B8-90F8-B69DE57BB396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBF8B0-11C8-4768-B5EB-C50E1FB90E67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="786">
   <si>
     <t>Project</t>
   </si>
@@ -2389,7 +2389,13 @@
     <t>Sum of AbsoluteRemovedPatterns</t>
   </si>
   <si>
-    <t>Sum of NumberOfRemovedPatterns(Absolute)</t>
+    <t xml:space="preserve"> AverageAdditionsPerIssueType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AverageRemovalsPerIssueType</t>
+  </si>
+  <si>
+    <t>Sum of NumberOfRemovedPatterns</t>
   </si>
 </sst>
 </file>
@@ -2532,7 +2538,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2724,8 +2730,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2934,6 +2958,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2979,7 +3021,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -2999,6 +3041,10 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="35" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3045,6 +3091,12 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -3095,12 +3147,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7267,8 +7313,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4971434" y="12702669"/>
-              <a:ext cx="6875588" cy="3978088"/>
+              <a:off x="4466609" y="12702669"/>
+              <a:ext cx="8418638" cy="3978088"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7414,7 +7460,7 @@
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="33">
+  <cacheFields count="35">
     <cacheField name="Project" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -7905,7 +7951,9 @@
     <cacheField name="SumOfPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
     <cacheField name="TotalPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
     <cacheField name="AbsoluteRemovedPatterns" numFmtId="0" formula="ABS(NumberOfRemovedPatterns)" databaseField="0"/>
-    <cacheField name="NumberOfRemovedPatterns(Absolute)" numFmtId="0" formula=" ABS(NumberOfRemovedPatterns )" databaseField="0"/>
+    <cacheField name="NumberOfRemovedPatterns(Absolute)" numFmtId="0" formula=" ABS(NumberOfRemovedPatterns)" databaseField="0"/>
+    <cacheField name="AverageChangesToPatterns" numFmtId="0" formula="TotalPatternChanges /CommitID" databaseField="0"/>
+    <cacheField name="AverageAdditionsPerIssueType" numFmtId="0" formula="TotalPatternChanges /CommitID" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -16973,9 +17021,546 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="35">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
+      <items count="11">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Sum of AbsoluteRemovedPatterns" fld="31" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B92:F98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="35">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="293">
+        <item x="127"/>
+        <item x="75"/>
+        <item x="42"/>
+        <item x="174"/>
+        <item x="48"/>
+        <item x="53"/>
+        <item x="45"/>
+        <item x="13"/>
+        <item x="230"/>
+        <item x="8"/>
+        <item x="194"/>
+        <item x="179"/>
+        <item x="177"/>
+        <item x="264"/>
+        <item x="70"/>
+        <item x="199"/>
+        <item x="167"/>
+        <item x="130"/>
+        <item x="266"/>
+        <item x="144"/>
+        <item x="202"/>
+        <item x="11"/>
+        <item x="166"/>
+        <item x="15"/>
+        <item x="277"/>
+        <item x="36"/>
+        <item x="110"/>
+        <item x="163"/>
+        <item x="152"/>
+        <item x="169"/>
+        <item x="2"/>
+        <item x="242"/>
+        <item x="111"/>
+        <item x="64"/>
+        <item x="88"/>
+        <item x="49"/>
+        <item x="128"/>
+        <item x="28"/>
+        <item x="212"/>
+        <item x="192"/>
+        <item x="119"/>
+        <item x="270"/>
+        <item x="245"/>
+        <item x="207"/>
+        <item x="121"/>
+        <item x="63"/>
+        <item x="261"/>
+        <item x="35"/>
+        <item x="14"/>
+        <item x="83"/>
+        <item x="134"/>
+        <item x="20"/>
+        <item x="252"/>
+        <item x="195"/>
+        <item x="116"/>
+        <item x="39"/>
+        <item x="38"/>
+        <item x="27"/>
+        <item x="175"/>
+        <item x="106"/>
+        <item x="156"/>
+        <item x="102"/>
+        <item x="101"/>
+        <item x="135"/>
+        <item x="285"/>
+        <item x="129"/>
+        <item x="224"/>
+        <item x="215"/>
+        <item x="187"/>
+        <item x="96"/>
+        <item x="288"/>
+        <item x="44"/>
+        <item x="286"/>
+        <item x="158"/>
+        <item x="244"/>
+        <item x="267"/>
+        <item x="114"/>
+        <item x="51"/>
+        <item x="235"/>
+        <item x="190"/>
+        <item x="6"/>
+        <item x="155"/>
+        <item x="209"/>
+        <item x="146"/>
+        <item x="280"/>
+        <item x="269"/>
+        <item x="246"/>
+        <item x="157"/>
+        <item x="55"/>
+        <item x="249"/>
+        <item x="108"/>
+        <item x="16"/>
+        <item x="160"/>
+        <item x="57"/>
+        <item x="99"/>
+        <item x="72"/>
+        <item x="238"/>
+        <item x="86"/>
+        <item x="196"/>
+        <item x="56"/>
+        <item x="182"/>
+        <item x="123"/>
+        <item x="76"/>
+        <item x="153"/>
+        <item x="112"/>
+        <item x="254"/>
+        <item x="243"/>
+        <item x="79"/>
+        <item x="122"/>
+        <item x="172"/>
+        <item x="191"/>
+        <item x="137"/>
+        <item x="24"/>
+        <item x="183"/>
+        <item x="165"/>
+        <item x="113"/>
+        <item x="91"/>
+        <item x="77"/>
+        <item x="273"/>
+        <item x="225"/>
+        <item x="197"/>
+        <item x="43"/>
+        <item x="241"/>
+        <item x="162"/>
+        <item x="73"/>
+        <item x="149"/>
+        <item x="164"/>
+        <item x="147"/>
+        <item x="143"/>
+        <item x="60"/>
+        <item x="223"/>
+        <item x="140"/>
+        <item x="208"/>
+        <item x="69"/>
+        <item x="255"/>
+        <item x="171"/>
+        <item x="188"/>
+        <item x="290"/>
+        <item x="282"/>
+        <item x="220"/>
+        <item x="21"/>
+        <item x="87"/>
+        <item x="204"/>
+        <item x="62"/>
+        <item x="200"/>
+        <item x="132"/>
+        <item x="236"/>
+        <item x="19"/>
+        <item x="25"/>
+        <item x="284"/>
+        <item x="234"/>
+        <item x="265"/>
+        <item x="278"/>
+        <item x="109"/>
+        <item x="211"/>
+        <item x="176"/>
+        <item x="205"/>
+        <item x="50"/>
+        <item x="29"/>
+        <item x="125"/>
+        <item x="22"/>
+        <item x="103"/>
+        <item x="7"/>
+        <item x="206"/>
+        <item x="90"/>
+        <item x="84"/>
+        <item x="104"/>
+        <item x="117"/>
+        <item x="12"/>
+        <item x="233"/>
+        <item x="71"/>
+        <item x="181"/>
+        <item x="279"/>
+        <item x="5"/>
+        <item x="82"/>
+        <item x="74"/>
+        <item x="240"/>
+        <item x="3"/>
+        <item x="228"/>
+        <item x="148"/>
+        <item x="253"/>
+        <item x="289"/>
+        <item x="287"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="251"/>
+        <item x="142"/>
+        <item x="40"/>
+        <item x="268"/>
+        <item x="126"/>
+        <item x="263"/>
+        <item x="78"/>
+        <item x="93"/>
+        <item x="189"/>
+        <item x="92"/>
+        <item x="47"/>
+        <item x="9"/>
+        <item x="46"/>
+        <item x="80"/>
+        <item x="30"/>
+        <item x="239"/>
+        <item x="95"/>
+        <item x="68"/>
+        <item x="198"/>
+        <item x="260"/>
+        <item x="247"/>
+        <item x="275"/>
+        <item x="33"/>
+        <item x="1"/>
+        <item x="201"/>
+        <item x="161"/>
+        <item x="250"/>
+        <item x="34"/>
+        <item x="173"/>
+        <item x="124"/>
+        <item x="216"/>
+        <item x="139"/>
+        <item x="61"/>
+        <item x="219"/>
+        <item x="26"/>
+        <item x="120"/>
+        <item x="85"/>
+        <item x="98"/>
+        <item x="258"/>
+        <item x="131"/>
+        <item x="231"/>
+        <item x="138"/>
+        <item x="203"/>
+        <item x="118"/>
+        <item x="185"/>
+        <item x="59"/>
+        <item x="184"/>
+        <item x="100"/>
+        <item x="272"/>
+        <item x="276"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="227"/>
+        <item x="133"/>
+        <item x="210"/>
+        <item x="248"/>
+        <item x="105"/>
+        <item x="145"/>
+        <item x="232"/>
+        <item x="52"/>
+        <item x="170"/>
+        <item x="229"/>
+        <item x="89"/>
+        <item x="97"/>
+        <item x="151"/>
+        <item x="141"/>
+        <item x="10"/>
+        <item x="291"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="178"/>
+        <item x="168"/>
+        <item x="222"/>
+        <item x="274"/>
+        <item x="180"/>
+        <item x="107"/>
+        <item x="262"/>
+        <item x="237"/>
+        <item x="37"/>
+        <item x="186"/>
+        <item x="4"/>
+        <item x="18"/>
+        <item x="115"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="41"/>
+        <item x="259"/>
+        <item x="226"/>
+        <item x="193"/>
+        <item x="218"/>
+        <item x="283"/>
+        <item x="271"/>
+        <item x="81"/>
+        <item x="54"/>
+        <item x="65"/>
+        <item x="31"/>
+        <item x="150"/>
+        <item x="94"/>
+        <item x="281"/>
+        <item x="221"/>
+        <item x="159"/>
+        <item x="154"/>
+        <item x="136"/>
+        <item x="217"/>
+        <item x="32"/>
+        <item x="58"/>
+        <item x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Sum of NumberOfRemovedPatterns" fld="32" baseField="6" baseItem="0"/>
+    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="6" baseItem="0" numFmtId="1"/>
+    <dataField name="Count of CommitID" fld="1" subtotal="count" baseField="6" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B71:C77" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="33">
+  <pivotFields count="35">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -17015,6 +17600,8 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -17061,10 +17648,10 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="B57:D66" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="33">
+  <pivotFields count="35">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
       <items count="293">
@@ -17500,6 +18087,8 @@
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="2"/>
@@ -17560,239 +18149,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="33">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
-      <items count="11">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of AbsoluteRemovedPatterns" fld="31" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B92:E98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="33">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of NumberOfRemovedPatterns(Absolute)" fld="32" baseField="0" baseItem="0"/>
-    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AC293" totalsRowShown="0">
   <autoFilter ref="A1:AC293" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -17809,23 +18165,23 @@
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="TimeToResolve(Days)"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NumberOfAddedPatterns"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NumberOfRemovedPatterns"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Abstract Factory" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Factory Method" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Singleton" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Adapter" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Bridge" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Composite" dataDxfId="11"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Decorator" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Facade" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Flyweight" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Proxy" dataDxfId="7"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Chain of Responsibility" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Mediator" dataDxfId="5"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Observer" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="State" dataDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Strategy" dataDxfId="2"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Template Method" dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Visitor" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Abstract Factory" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Factory Method" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Singleton" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Adapter" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Bridge" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Composite" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Decorator" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Facade" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Flyweight" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Proxy" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Chain of Responsibility" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Mediator" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Observer" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="State" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Strategy" dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Template Method" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Visitor" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17835,8 +18191,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00C4A24C-F4A7-4272-A428-C9904738F93F}" name="Table3" displayName="Table3" ref="E57:F65" totalsRowShown="0">
   <autoFilter ref="E57:F65" xr:uid="{EB3308BB-A406-42BA-A76D-F94720BFCCA3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CB378E6D-067E-4D65-BC80-38A6B0CE5641}" name="Count of CommitID" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{9C45E57F-72E8-4004-9367-2BB9F710DAA0}" name="PatternChanges" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{CB378E6D-067E-4D65-BC80-38A6B0CE5641}" name="Count of CommitID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9C45E57F-72E8-4004-9367-2BB9F710DAA0}" name="PatternChanges" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -31303,30 +31659,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92:H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -32087,7 +32442,7 @@
         <v>89.670103092783506</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>770</v>
       </c>
@@ -32095,13 +32450,22 @@
         <v>772</v>
       </c>
       <c r="D92" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="E92" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>778</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>783</v>
+      </c>
+      <c r="H92" s="17" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>46</v>
       </c>
@@ -32111,11 +32475,22 @@
       <c r="D93" s="4">
         <v>43</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93" s="5">
         <v>94</v>
       </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="5">
+        <v>30</v>
+      </c>
+      <c r="G93" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Bug")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Bug")</f>
+        <v>1.7</v>
+      </c>
+      <c r="H93" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Bug")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Bug")</f>
+        <v>1.4333333333333333</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>54</v>
       </c>
@@ -32125,11 +32500,22 @@
       <c r="D94" s="4">
         <v>96</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E94" s="5">
         <v>182</v>
       </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="5">
+        <v>27</v>
+      </c>
+      <c r="G94" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Improvement")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Improvement")</f>
+        <v>3.1851851851851851</v>
+      </c>
+      <c r="H94" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Improvement")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Improvement")</f>
+        <v>3.5555555555555554</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>91</v>
       </c>
@@ -32139,11 +32525,22 @@
       <c r="D95" s="4">
         <v>80</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E95" s="5">
         <v>237</v>
       </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="5">
+        <v>31</v>
+      </c>
+      <c r="G95" s="20">
+        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","New Feature")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","New Feature")</f>
+        <v>5.064516129032258</v>
+      </c>
+      <c r="H95" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","New Feature")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","New Feature")</f>
+        <v>2.5806451612903225</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
         <v>144</v>
       </c>
@@ -32153,11 +32550,22 @@
       <c r="D96" s="4">
         <v>41</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96" s="5">
         <v>73</v>
       </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="5">
+        <v>7</v>
+      </c>
+      <c r="G96" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Task")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Task")</f>
+        <v>4.5714285714285712</v>
+      </c>
+      <c r="H96" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Task")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Task")</f>
+        <v>5.8571428571428568</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
         <v>70</v>
       </c>
@@ -32167,11 +32575,22 @@
       <c r="D97" s="4">
         <v>0</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E97" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F97" s="5">
+        <v>2</v>
+      </c>
+      <c r="G97" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Test")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Test")</f>
+        <v>1</v>
+      </c>
+      <c r="H97" s="19">
+        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Test")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Test")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>771</v>
       </c>
@@ -32181,9 +32600,14 @@
       <c r="D98" s="4">
         <v>260</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98" s="5">
         <v>588</v>
       </c>
+      <c r="F98" s="5">
+        <v>97</v>
+      </c>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed all the diagrams and information regarding the report
</commit_message>
<xml_diff>
--- a/Documentation/mina-finalResults-graphs.xlsx
+++ b/Documentation/mina-finalResults-graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitRepos\Internship_RuG_2020\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBF8B0-11C8-4768-B5EB-C50E1FB90E67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1263A15B-35FD-4CB0-96D5-3C76DC29E591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mina-finalResults-CSV" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="787">
   <si>
     <t>Project</t>
   </si>
@@ -2383,19 +2383,22 @@
     <t>Average of TimeToResolve(Days)</t>
   </si>
   <si>
-    <t>Sum of TotalPatternChanges</t>
-  </si>
-  <si>
     <t>Sum of AbsoluteRemovedPatterns</t>
   </si>
   <si>
-    <t xml:space="preserve"> AverageAdditionsPerIssueType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AverageRemovalsPerIssueType</t>
-  </si>
-  <si>
-    <t>Sum of NumberOfRemovedPatterns</t>
+    <t>Number of Issues</t>
+  </si>
+  <si>
+    <t>Added Patterns</t>
+  </si>
+  <si>
+    <t>Removed Patterns</t>
+  </si>
+  <si>
+    <t>Relative Added Patterns</t>
+  </si>
+  <si>
+    <t>Relative Removed Patterns</t>
   </si>
 </sst>
 </file>
@@ -4975,6 +4978,492 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Relative changes</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to the patterns per issue type</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphs and Tables'!$F$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative Added Patterns</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphs and Tables'!$B$93:$B$97</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Bug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Improvement</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>New Feature</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Task</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphs and Tables'!$F$93:$F$97</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1851851851851851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.064516129032258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5714285714285712</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DCF-4159-9708-D30D289BCAC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphs and Tables'!$G$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative Removed Patterns</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphs and Tables'!$B$93:$B$97</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Bug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Improvement</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>New Feature</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Task</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphs and Tables'!$G$93:$G$97</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.4333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5806451612903225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8571428571428568</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1DCF-4159-9708-D30D289BCAC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="796581311"/>
+        <c:axId val="1089989087"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="796581311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1089989087"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1089989087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pattern Changes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="796581311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -5042,8 +5531,61 @@
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Days</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Days</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
   </cx:chart>
@@ -5184,6 +5726,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7264,6 +7846,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7313,8 +8398,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4466609" y="12702669"/>
-              <a:ext cx="8418638" cy="3978088"/>
+              <a:off x="4314209" y="12702669"/>
+              <a:ext cx="5923088" cy="3978088"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7447,6 +8532,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5603</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>34738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409015</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>110938</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F776D0EE-0022-4979-895C-BEC852B830CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7952,8 +9073,8 @@
     <cacheField name="TotalPatternChanges" numFmtId="0" formula="NumberOfAddedPatterns+ ABS(NumberOfRemovedPatterns)" databaseField="0"/>
     <cacheField name="AbsoluteRemovedPatterns" numFmtId="0" formula="ABS(NumberOfRemovedPatterns)" databaseField="0"/>
     <cacheField name="NumberOfRemovedPatterns(Absolute)" numFmtId="0" formula=" ABS(NumberOfRemovedPatterns)" databaseField="0"/>
-    <cacheField name="AverageChangesToPatterns" numFmtId="0" formula="TotalPatternChanges /CommitID" databaseField="0"/>
-    <cacheField name="AverageAdditionsPerIssueType" numFmtId="0" formula="TotalPatternChanges /CommitID" databaseField="0"/>
+    <cacheField name="AverageChangesToPatterns" numFmtId="0" formula="TotalPatternChanges/CommitID" databaseField="0"/>
+    <cacheField name="AverageAdditionsPerIssueType" numFmtId="0" formula="TotalPatternChanges/CommitID" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -17021,7 +18142,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="B33:D42" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="35">
     <pivotField showAll="0"/>
@@ -17154,8 +18275,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B92:F98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B92:E98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="35">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
@@ -17493,7 +18614,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -17525,7 +18646,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="3">
     <i>
       <x/>
     </i>
@@ -17535,15 +18656,11 @@
     <i i="2">
       <x v="2"/>
     </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
   </colItems>
-  <dataFields count="4">
-    <dataField name="Sum of NumberOfAddedPatterns" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of NumberOfRemovedPatterns" fld="32" baseField="6" baseItem="0"/>
-    <dataField name="Sum of TotalPatternChanges" fld="30" baseField="6" baseItem="0" numFmtId="1"/>
-    <dataField name="Count of CommitID" fld="1" subtotal="count" baseField="6" baseItem="0" numFmtId="1"/>
+  <dataFields count="3">
+    <dataField name="Added Patterns" fld="10" baseField="6" baseItem="0"/>
+    <dataField name="Removed Patterns" fld="32" baseField="6" baseItem="0"/>
+    <dataField name="Number of Issues" fld="1" subtotal="count" baseField="6" baseItem="0" numFmtId="1"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -17558,7 +18675,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E65CE58-CE72-4B1F-B239-0887C714A660}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B71:C77" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="35">
     <pivotField showAll="0"/>
@@ -17649,7 +18766,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showError="1" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="B57:D66" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="35">
     <pivotField showAll="0"/>
@@ -31659,17 +32776,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92:H98"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="30.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -32120,7 +33237,7 @@
         <v>772</v>
       </c>
       <c r="D33" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -32442,30 +33559,27 @@
         <v>89.670103092783506</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>770</v>
       </c>
       <c r="C92" t="s">
-        <v>772</v>
+        <v>783</v>
       </c>
       <c r="D92" t="s">
+        <v>784</v>
+      </c>
+      <c r="E92" t="s">
+        <v>782</v>
+      </c>
+      <c r="F92" s="17" t="s">
         <v>785</v>
       </c>
-      <c r="E92" t="s">
-        <v>781</v>
-      </c>
-      <c r="F92" t="s">
-        <v>778</v>
-      </c>
       <c r="G92" s="17" t="s">
-        <v>783</v>
-      </c>
-      <c r="H92" s="17" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>46</v>
       </c>
@@ -32476,21 +33590,18 @@
         <v>43</v>
       </c>
       <c r="E93" s="5">
-        <v>94</v>
-      </c>
-      <c r="F93" s="5">
         <v>30</v>
       </c>
+      <c r="F93" s="19">
+        <f>GETPIVOTDATA("Added Patterns",$B$92,"IssueType","Bug")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Bug")</f>
+        <v>1.7</v>
+      </c>
       <c r="G93" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Bug")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Bug")</f>
-        <v>1.7</v>
-      </c>
-      <c r="H93" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Bug")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Bug")</f>
+        <f>GETPIVOTDATA("Removed Patterns",$B$92,"IssueType","Bug")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Bug")</f>
         <v>1.4333333333333333</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>54</v>
       </c>
@@ -32501,21 +33612,18 @@
         <v>96</v>
       </c>
       <c r="E94" s="5">
-        <v>182</v>
-      </c>
-      <c r="F94" s="5">
         <v>27</v>
       </c>
+      <c r="F94" s="19">
+        <f>GETPIVOTDATA("Added Patterns",$B$92,"IssueType","Improvement")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Improvement")</f>
+        <v>3.1851851851851851</v>
+      </c>
       <c r="G94" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Improvement")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Improvement")</f>
-        <v>3.1851851851851851</v>
-      </c>
-      <c r="H94" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Improvement")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Improvement")</f>
+        <f>GETPIVOTDATA("Removed Patterns",$B$92,"IssueType","Improvement")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Improvement")</f>
         <v>3.5555555555555554</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>91</v>
       </c>
@@ -32526,21 +33634,18 @@
         <v>80</v>
       </c>
       <c r="E95" s="5">
-        <v>237</v>
-      </c>
-      <c r="F95" s="5">
         <v>31</v>
       </c>
-      <c r="G95" s="20">
-        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","New Feature")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","New Feature")</f>
+      <c r="F95" s="20">
+        <f>GETPIVOTDATA("Added Patterns",$B$92,"IssueType","New Feature")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","New Feature")</f>
         <v>5.064516129032258</v>
       </c>
-      <c r="H95" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","New Feature")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","New Feature")</f>
+      <c r="G95" s="19">
+        <f>GETPIVOTDATA("Removed Patterns",$B$92,"IssueType","New Feature")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","New Feature")</f>
         <v>2.5806451612903225</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
         <v>144</v>
       </c>
@@ -32551,21 +33656,18 @@
         <v>41</v>
       </c>
       <c r="E96" s="5">
-        <v>73</v>
-      </c>
-      <c r="F96" s="5">
         <v>7</v>
       </c>
+      <c r="F96" s="19">
+        <f>GETPIVOTDATA("Added Patterns",$B$92,"IssueType","Task")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Task")</f>
+        <v>4.5714285714285712</v>
+      </c>
       <c r="G96" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Task")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Task")</f>
-        <v>4.5714285714285712</v>
-      </c>
-      <c r="H96" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Task")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Task")</f>
+        <f>GETPIVOTDATA("Removed Patterns",$B$92,"IssueType","Task")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Task")</f>
         <v>5.8571428571428568</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
         <v>70</v>
       </c>
@@ -32578,19 +33680,16 @@
       <c r="E97" s="5">
         <v>2</v>
       </c>
-      <c r="F97" s="5">
-        <v>2</v>
+      <c r="F97" s="19">
+        <f>GETPIVOTDATA("Added Patterns",$B$92,"IssueType","Test")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Test")</f>
+        <v>1</v>
       </c>
       <c r="G97" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfAddedPatterns",$B$92,"IssueType","Test")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Test")</f>
-        <v>1</v>
-      </c>
-      <c r="H97" s="19">
-        <f>GETPIVOTDATA("Sum of NumberOfRemovedPatterns",$B$92,"IssueType","Test")/GETPIVOTDATA("Count of CommitID",$B$92,"IssueType","Test")</f>
+        <f>GETPIVOTDATA("Removed Patterns",$B$92,"IssueType","Test")/GETPIVOTDATA("Number of Issues",$B$92,"IssueType","Test")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>771</v>
       </c>
@@ -32601,13 +33700,10 @@
         <v>260</v>
       </c>
       <c r="E98" s="5">
-        <v>588</v>
-      </c>
-      <c r="F98" s="5">
         <v>97</v>
       </c>
+      <c r="F98" s="18"/>
       <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>